<commit_message>
RMD : news index fix; reduce space between title and article body
</commit_message>
<xml_diff>
--- a/RMD/input/news.xlsx
+++ b/RMD/input/news.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16425"/>
   </bookViews>
   <sheets>
-    <sheet name="international" sheetId="1" r:id="rId4"/>
-    <sheet name="china" sheetId="2" r:id="rId5"/>
+    <sheet name="international" sheetId="1" r:id="rId1"/>
+    <sheet name="china" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Pub</t>
   </si>
@@ -26,50 +29,119 @@
     <t xml:space="preserve">有线电视新闻网(CNN) </t>
   </si>
   <si>
-    <t>特朗普签署2万亿美元的经济援助法案</t>
-  </si>
-  <si>
-    <t>当地时间3月27日下午4时30分，美国总统特朗普发推文称他签署了美国有史以来金额最大的经济援助法 案(CARES法)，该法案总救济金额为2.2万亿美元，将为美国的家庭、工人和企业提供紧急救援。</t>
-  </si>
-  <si>
-    <t>BBC</t>
-  </si>
-  <si>
-    <t>新闻</t>
-  </si>
-  <si>
     <t>pub</t>
   </si>
   <si>
     <t>Content</t>
+  </si>
+  <si>
+    <t>北京时间4月2日，外交部副部长马兆旭表示，中国在3月安排了9次包机，将1457名海 外的中国公民带回国，其中包括来自伊朗，意大利等国家的海外留学生。</t>
+  </si>
+  <si>
+    <t>中国日报(China Daily)</t>
+  </si>
+  <si>
+    <t>中国安排9次包机从海外接回1457人</t>
+  </si>
+  <si>
+    <t>李文亮江学庆等14人获评烈士</t>
+  </si>
+  <si>
+    <t>财新网(Caixin.com)</t>
+  </si>
+  <si>
+    <t>北京时间4月2日，湖北省人民政府评定王兵、冯效林、江学庆、刘智明、李文亮、张 抗美、肖俊、吴涌、柳帆、夏思思、黄文军、梅仲明、彭银华、廖建军等14名牺牲在 新冠肺炎疫情防控一线人员为首批烈士。</t>
+  </si>
+  <si>
+    <t>英国广播公司(BBC)</t>
+  </si>
+  <si>
+    <t>有线电视新闻网(CNN)</t>
+  </si>
+  <si>
+    <t>环球时报(Global Times)</t>
+  </si>
+  <si>
+    <t>世界银行宣布19亿美元紧急资金</t>
+  </si>
+  <si>
+    <t>120万个N95口罩正从中国运往美国</t>
+  </si>
+  <si>
+    <t>当地时间4月1日，新英格兰爱国者队的飞机从中国深圳出发，运载120万个N95口罩前 往美国，预计将于4月2日达到波士顿洛根机场。</t>
+  </si>
+  <si>
+    <t>美国总统特朗普启用国防生产法，点名七家公司生产呼吸机</t>
+  </si>
+  <si>
+    <t>当地时间4月2日，白宫发布声明称，美国总统特朗普下令全面启用国防生产法，并在 声明中点名希望通用电气、美敦力、飞利浦等七家美国公司可以通过此法案更顺利地 获取生产呼吸机所需的材料。</t>
+  </si>
+  <si>
+    <t>意大利医护人员感染超1万</t>
+  </si>
+  <si>
+    <t>当地时间4月2日，意大利外科和牙科医生联合会发布公告称，意大利自疫情爆发以来 因感染新冠肺炎去世的医生达69人;另据卫生医疗行业协会通报，意大利目前感染新 冠肺炎的医护人员超过1万例。</t>
+  </si>
+  <si>
+    <t>澳大利亚将有100万家庭获得免费托儿服务</t>
+  </si>
+  <si>
+    <t>当地时间4月2日，澳大利亚总理斯科特·莫里森宣布，由于新冠肺炎疫情影响，澳大 利亚计划为约100万个家庭提供免费托儿服务。</t>
+  </si>
+  <si>
+    <t>据4月2日的报道称，世界银行已启动了一项19亿美元的应急基金，以帮助25个国家应 对新冠病毒大流行。 其中，印度将获得最大的一笔资金(10亿美元)来改善新冠筛 查、追踪和实验室诊断，资金还将用于购买个人防护设备和建立隔离病房。</t>
+  </si>
+  <si>
+    <t>非洲疾控中心(Africa CDC)</t>
+  </si>
+  <si>
+    <t>非洲新冠肺炎超7000例 蔓延50国</t>
+  </si>
+  <si>
+    <t>截至非洲东部时间4月3日17时，非洲共有50国出现新冠肺炎疫情，总数达7123例，死
+亡289例，治愈592例。</t>
+  </si>
+  <si>
+    <t>新闻来源</t>
+  </si>
+  <si>
+    <t>新闻标题</t>
+  </si>
+  <si>
+    <t>新闻内容</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -100,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -165,17 +237,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="10"/>
       </left>
@@ -184,196 +245,50 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -384,28 +299,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -607,7 +579,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -626,7 +598,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -656,7 +628,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -682,7 +654,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -708,7 +680,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -734,7 +706,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -760,7 +732,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -786,7 +758,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +784,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -838,7 +810,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -864,7 +836,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -877,9 +849,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -896,7 +874,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -915,7 +893,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -941,7 +919,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -967,7 +945,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -993,7 +971,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1019,7 +997,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1023,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1071,7 +1049,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1097,7 +1075,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1123,7 +1101,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,7 +1127,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1162,9 +1140,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1178,7 +1162,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1197,7 +1181,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1211,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1237,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1263,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1289,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1315,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1357,7 +1341,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,7 +1367,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1409,7 +1393,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1435,7 +1419,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1448,155 +1432,149 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="20" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="63" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="147.852" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.35156" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="80.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="8.28515625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="4"/>
     </row>
-    <row r="2" ht="20" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:5" ht="60" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="60" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="60" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4"/>
     </row>
-    <row r="3" ht="20" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="5" spans="1:5" ht="60" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="60" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4"/>
     </row>
-    <row r="4" ht="20" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+    <row r="7" spans="1:5" ht="60" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
     </row>
-    <row r="5" ht="14.75" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="14.75" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="14.75" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="14.75" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="14.75" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="14.75" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
+    <row r="8" spans="1:5" ht="60" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1604,141 +1582,78 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="14.1" customHeight="1"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="18" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="80.7109375" style="3" customWidth="1"/>
+    <col min="4" max="6" width="16.28515625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="16.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.35" customHeight="1">
-      <c r="A1" t="s" s="19">
+    <row r="1" spans="1:3" ht="14.25">
+      <c r="A1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s" s="19">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="C3" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" ht="14.7" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+    <row r="4" spans="1:3" ht="60" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" ht="14.7" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-    </row>
-    <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-    </row>
-    <row r="9" ht="14.35" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-    </row>
+    <row r="5" spans="1:3" ht="74.25" customHeight="1"/>
+    <row r="6" spans="1:3" ht="74.25" customHeight="1"/>
+    <row r="7" spans="1:3" ht="74.25" customHeight="1"/>
+    <row r="8" spans="1:3" ht="74.25" customHeight="1"/>
+    <row r="9" spans="1:3" ht="74.25" customHeight="1"/>
+    <row r="10" spans="1:3" ht="74.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>